<commit_message>
Excel Test Driver and Model changes
</commit_message>
<xml_diff>
--- a/dataloader/src/test/resources/TestDriver/TestModel_V2/Test.xlsx
+++ b/dataloader/src/test/resources/TestDriver/TestModel_V2/Test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t xml:space="preserve">Steps</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">CONFIGURATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTRIBUTE</t>
   </si>
   <si>
     <t xml:space="preserve">ACTIVITY_UPLOAD</t>
@@ -291,7 +294,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -341,24 +344,27 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>44592</v>
@@ -366,21 +372,21 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>44593</v>
@@ -388,21 +394,21 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>44594</v>
@@ -410,21 +416,21 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>44595</v>
@@ -432,21 +438,21 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>44596</v>
@@ -454,10 +460,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>44597</v>
@@ -465,21 +471,21 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>44598</v>

</xml_diff>